<commit_message>
更改 AppiumDriver 为 AppiumXMDriver
</commit_message>
<xml_diff>
--- a/testCase/163mailTest/module.xlsx
+++ b/testCase/163mailTest/module.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>YES</t>
   </si>
@@ -69,10 +69,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>com.netease.mail:id/editor_email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ById</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -130,6 +126,14 @@
   </si>
   <si>
     <t>com.netease.mail:id/editor_password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ByAndroidUIAutomator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>new UiSelector().text("邮箱帐号")</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -574,7 +578,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -584,7 +588,7 @@
     <col min="3" max="3" width="16.125" style="4" customWidth="1"/>
     <col min="4" max="4" width="16.875" style="4" customWidth="1"/>
     <col min="5" max="5" width="13.75" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.75" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.875" style="4" customWidth="1"/>
     <col min="7" max="7" width="29.625" style="4" customWidth="1"/>
     <col min="8" max="8" width="9.25" style="4" customWidth="1"/>
     <col min="9" max="9" width="21.25" style="4" customWidth="1"/>
@@ -634,25 +638,25 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H2" s="1">
         <v>10</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" s="1"/>
     </row>
@@ -664,25 +668,25 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1">
         <v>10</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -691,24 +695,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J4" s="1"/>
     </row>

</xml_diff>